<commit_message>
Build a token string
</commit_message>
<xml_diff>
--- a/PocketNurseTest/ErrorRequest1.xlsx
+++ b/PocketNurseTest/ErrorRequest1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccaannburton/Projects/PocketNurse/PocketNurseTest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccaannburton/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED278691-0C3C-7C46-8978-F1C5A5ABAD21}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{188B8BC1-56A5-7D4F-B5BE-515107AB0A0A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="23000" windowHeight="9520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="23000" windowHeight="9520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Session" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>Allergies</t>
   </si>
@@ -136,24 +136,9 @@
     <t>ondansetron</t>
   </si>
   <si>
-    <t>Session</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Area</t>
-  </si>
-  <si>
     <t>Wisconsin</t>
   </si>
   <si>
-    <t>Madison</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -164,15 +149,33 @@
   </si>
   <si>
     <t>Medical Record Number</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Site ID</t>
+  </si>
+  <si>
+    <t>SVR</t>
+  </si>
+  <si>
+    <t>Console</t>
+  </si>
+  <si>
+    <t>Omni ID</t>
+  </si>
+  <si>
+    <t>Omnicell</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -224,12 +227,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,41 +574,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A910568-28D3-FF46-AA0D-B66B4AE7533A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>43221.458333333336</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -617,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -631,16 +635,16 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>

</xml_diff>